<commit_message>
Ajusta merge de coordenadores e filtros (PT + % + correções)
</commit_message>
<xml_diff>
--- a/data/Base_Coordenadores.xlsx
+++ b/data/Base_Coordenadores.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jet Express\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jet Express\Desktop\Retenção Streamlit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0689C6-ECCC-4167-ADBC-9D4A4A56DB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C189E8B0-F0E3-49D1-987D-EE0876B0A7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base - Atulizada" sheetId="2" r:id="rId1"/>
@@ -453,9 +453,6 @@
     <t>Nome da base</t>
   </si>
   <si>
-    <t>Coordenadores</t>
-  </si>
-  <si>
     <t>UF</t>
   </si>
   <si>
@@ -712,6 +709,9 @@
   </si>
   <si>
     <t>Jose Marlon</t>
+  </si>
+  <si>
+    <t>Coordenador</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1106,7 @@
   <dimension ref="A1:D198"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1120,7 +1120,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>112</v>
@@ -1129,7 +1129,7 @@
         <v>137</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>138</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1140,10 +1140,10 @@
         <v>104</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1157,7 +1157,7 @@
         <v>62</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1168,10 +1168,10 @@
         <v>104</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1185,7 +1185,7 @@
         <v>81</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1199,7 +1199,7 @@
         <v>77</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1213,7 +1213,7 @@
         <v>76</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1227,7 +1227,7 @@
         <v>120</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1241,7 +1241,7 @@
         <v>68</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1255,7 +1255,7 @@
         <v>67</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1269,7 +1269,7 @@
         <v>66</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1283,7 +1283,7 @@
         <v>65</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1297,7 +1297,7 @@
         <v>99</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1308,10 +1308,10 @@
         <v>104</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1325,21 +1325,21 @@
         <v>43</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1350,15 +1350,15 @@
         <v>104</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>104</v>
@@ -1367,12 +1367,12 @@
         <v>80</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>104</v>
@@ -1381,26 +1381,26 @@
         <v>79</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>104</v>
@@ -1409,12 +1409,12 @@
         <v>122</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>104</v>
@@ -1423,12 +1423,12 @@
         <v>123</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>104</v>
@@ -1437,12 +1437,12 @@
         <v>61</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>104</v>
@@ -1451,12 +1451,12 @@
         <v>54</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>104</v>
@@ -1465,12 +1465,12 @@
         <v>48</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>104</v>
@@ -1479,7 +1479,7 @@
         <v>47</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1493,7 +1493,7 @@
         <v>87</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1507,7 +1507,7 @@
         <v>83</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1521,7 +1521,7 @@
         <v>82</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1535,7 +1535,7 @@
         <v>69</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1549,7 +1549,7 @@
         <v>121</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1560,10 +1560,10 @@
         <v>104</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1574,10 +1574,10 @@
         <v>104</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1588,10 +1588,10 @@
         <v>104</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1605,7 +1605,7 @@
         <v>59</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1619,7 +1619,7 @@
         <v>58</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1633,7 +1633,7 @@
         <v>52</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1647,32 +1647,32 @@
         <v>51</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>114</v>
@@ -1680,13 +1680,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>114</v>
@@ -1694,7 +1694,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>0</v>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>0</v>
@@ -1722,7 +1722,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>0</v>
@@ -1736,7 +1736,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>0</v>
@@ -1750,7 +1750,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>0</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>0</v>
@@ -1778,7 +1778,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>0</v>
@@ -1792,13 +1792,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>114</v>
@@ -1806,13 +1806,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>114</v>
@@ -1820,7 +1820,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>0</v>
@@ -1834,7 +1834,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>0</v>
@@ -1910,7 +1910,7 @@
         <v>104</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>106</v>
@@ -1932,7 +1932,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>104</v>
@@ -1946,13 +1946,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>116</v>
@@ -1980,7 +1980,7 @@
         <v>0</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>116</v>
@@ -1991,10 +1991,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>116</v>
@@ -2005,10 +2005,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>116</v>
@@ -2019,10 +2019,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>116</v>
@@ -2036,7 +2036,7 @@
         <v>0</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>116</v>
@@ -2050,7 +2050,7 @@
         <v>0</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>116</v>
@@ -2075,10 +2075,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>116</v>
@@ -2086,7 +2086,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>0</v>
@@ -2100,13 +2100,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>116</v>
@@ -2114,13 +2114,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>116</v>
@@ -2128,13 +2128,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>116</v>
@@ -2142,7 +2142,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>0</v>
@@ -2162,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>117</v>
@@ -2176,7 +2176,7 @@
         <v>0</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>117</v>
@@ -2344,7 +2344,7 @@
         <v>0</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>117</v>
@@ -2358,7 +2358,7 @@
         <v>0</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>117</v>
@@ -2400,7 +2400,7 @@
         <v>0</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>117</v>
@@ -2470,7 +2470,7 @@
         <v>0</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>117</v>
@@ -2478,35 +2478,35 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>104</v>
@@ -2515,40 +2515,40 @@
         <v>91</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>104</v>
@@ -2557,12 +2557,12 @@
         <v>89</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>104</v>
@@ -2571,7 +2571,7 @@
         <v>129</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -2579,13 +2579,13 @@
         <v>104</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -2593,18 +2593,18 @@
         <v>104</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>104</v>
@@ -2613,12 +2613,12 @@
         <v>90</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>104</v>
@@ -2627,12 +2627,12 @@
         <v>124</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>104</v>
@@ -2641,12 +2641,12 @@
         <v>98</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>104</v>
@@ -2655,12 +2655,12 @@
         <v>97</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>104</v>
@@ -2669,32 +2669,32 @@
         <v>88</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>113</v>
@@ -2702,13 +2702,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>113</v>
@@ -2716,13 +2716,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>113</v>
@@ -2730,13 +2730,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>113</v>
@@ -2744,13 +2744,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>113</v>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>0</v>
@@ -2772,13 +2772,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>113</v>
@@ -2786,7 +2786,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>0</v>
@@ -2800,13 +2800,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>113</v>
@@ -2814,13 +2814,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>113</v>
@@ -2828,13 +2828,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>113</v>
@@ -2842,7 +2842,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>104</v>
@@ -2859,10 +2859,10 @@
         <v>0</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>113</v>
@@ -2873,10 +2873,10 @@
         <v>0</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>113</v>
@@ -2884,13 +2884,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>113</v>
@@ -2898,13 +2898,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>113</v>
@@ -2912,13 +2912,13 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>119</v>
@@ -2926,7 +2926,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>0</v>
@@ -2940,7 +2940,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>0</v>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>0</v>
@@ -2968,7 +2968,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>0</v>
@@ -2982,13 +2982,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>119</v>
@@ -2996,7 +2996,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>0</v>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>0</v>
@@ -3024,13 +3024,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>119</v>
@@ -3038,7 +3038,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>0</v>
@@ -3052,7 +3052,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>0</v>
@@ -3066,7 +3066,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>0</v>
@@ -3080,7 +3080,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>0</v>
@@ -3094,7 +3094,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>0</v>
@@ -3108,13 +3108,13 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>119</v>
@@ -3122,13 +3122,13 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>115</v>
@@ -3136,13 +3136,13 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>115</v>
@@ -3150,13 +3150,13 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>115</v>
@@ -3164,7 +3164,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>0</v>
@@ -3178,7 +3178,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>0</v>
@@ -3192,7 +3192,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>0</v>
@@ -3206,7 +3206,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>0</v>
@@ -3220,13 +3220,13 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B151" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>115</v>
@@ -3234,7 +3234,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>0</v>
@@ -3248,7 +3248,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B153" s="3" t="s">
         <v>0</v>
@@ -3262,7 +3262,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B154" s="3" t="s">
         <v>0</v>
@@ -3276,7 +3276,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B155" s="3" t="s">
         <v>0</v>
@@ -3290,7 +3290,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>0</v>
@@ -3304,7 +3304,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>0</v>
@@ -3318,7 +3318,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>0</v>
@@ -3332,7 +3332,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B159" s="3" t="s">
         <v>0</v>
@@ -3346,13 +3346,13 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>115</v>
@@ -3366,7 +3366,7 @@
         <v>104</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>105</v>
@@ -3492,7 +3492,7 @@
         <v>104</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D170" s="3" t="s">
         <v>105</v>
@@ -3506,7 +3506,7 @@
         <v>104</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D171" s="3" t="s">
         <v>105</v>
@@ -3520,7 +3520,7 @@
         <v>104</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D172" s="3" t="s">
         <v>105</v>
@@ -3534,7 +3534,7 @@
         <v>104</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D173" s="3" t="s">
         <v>105</v>
@@ -3562,7 +3562,7 @@
         <v>104</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D175" s="3" t="s">
         <v>105</v>
@@ -3590,7 +3590,7 @@
         <v>104</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D177" s="3" t="s">
         <v>105</v>
@@ -3738,7 +3738,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B188" s="3" t="s">
         <v>104</v>
@@ -3752,7 +3752,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>104</v>
@@ -3766,13 +3766,13 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B190" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D190" s="3" t="s">
         <v>105</v>
@@ -3780,13 +3780,13 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B191" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D191" s="3" t="s">
         <v>118</v>
@@ -3794,7 +3794,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B192" s="3" t="s">
         <v>0</v>
@@ -3808,7 +3808,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B193" s="3" t="s">
         <v>0</v>
@@ -3822,7 +3822,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B194" s="3" t="s">
         <v>0</v>
@@ -3836,7 +3836,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B195" s="3" t="s">
         <v>0</v>
@@ -3850,13 +3850,13 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B196" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D196" s="3" t="s">
         <v>118</v>
@@ -3864,13 +3864,13 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B197" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D197" s="3" t="s">
         <v>118</v>
@@ -3878,7 +3878,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B198" s="3" t="s">
         <v>0</v>

</xml_diff>